<commit_message>
Endret tekst på norsk under "Vis mer"
</commit_message>
<xml_diff>
--- a/code_table_endringer.xlsx
+++ b/code_table_endringer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\4168_Resources\System- og programvareforvaltning\Oria\Code tables\Norsk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\4168_Resources\System- og programvareforvaltning\Oria\UI\Code tables\Norsk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -179,7 +179,7 @@
     <t>Include material your institution doesn't have access to</t>
   </si>
   <si>
-    <t>Inkluder materiale ditt bibliotek ikke har tilgang til</t>
+    <t>Inkluder materiale biblioteket ikke har elektronisk tilgang til</t>
   </si>
 </sst>
 </file>
@@ -521,7 +521,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>